<commit_message>
HG23 and RS23 data update
</commit_message>
<xml_diff>
--- a/projects_2023/JI23_FIN_SA/JI23_FIN_SA_Ft_data_7.xlsx
+++ b/projects_2023/JI23_FIN_SA/JI23_FIN_SA_Ft_data_7.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guest\Desktop\Josh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lab-admin\Documents\GitHub\HAL_data\projects_2023\JI23_FIN_SA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEDCBFD-1411-4355-B902-EF3CBF304740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F855533-CC94-430D-ABB9-98870ABEFB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{3F36359C-009B-4BEB-900D-FB1CD279B6D4}"/>
   </bookViews>
@@ -330,7 +330,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +372,13 @@
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -393,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -414,6 +421,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C343A43-C8CF-4105-8B1D-CAF7EB9B0B91}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,45 +1102,45 @@
       <c r="A22" t="s">
         <v>28</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="10">
         <v>7</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="10">
         <v>343.91</v>
       </c>
-      <c r="E22">
-        <v>345.58</v>
-      </c>
-      <c r="F22">
+      <c r="E22" s="10">
+        <v>319.32</v>
+      </c>
+      <c r="F22" s="10">
         <v>100.91</v>
       </c>
-      <c r="G22">
-        <v>102.54</v>
+      <c r="G22" s="10">
+        <v>88.12</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="10">
         <v>6</v>
       </c>
-      <c r="D23">
-        <v>354.39</v>
-      </c>
-      <c r="E23">
+      <c r="D23" s="10">
+        <v>311.66000000000003</v>
+      </c>
+      <c r="E23" s="10">
         <v>357.16</v>
       </c>
-      <c r="F23">
-        <v>116.7</v>
-      </c>
-      <c r="G23">
+      <c r="F23" s="10">
+        <v>116.73</v>
+      </c>
+      <c r="G23" s="10">
         <v>142</v>
       </c>
       <c r="H23">
@@ -1143,22 +1151,22 @@
       <c r="A24" t="s">
         <v>30</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="10">
         <v>6</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="10">
         <v>220.27</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="10">
         <v>219.69</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="10">
         <v>124.65</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="10">
         <v>86.78</v>
       </c>
       <c r="H24">
@@ -1169,22 +1177,22 @@
       <c r="A25" t="s">
         <v>31</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="10">
         <v>6</v>
       </c>
-      <c r="D25">
-        <v>305.75</v>
-      </c>
-      <c r="E25">
-        <v>301.99</v>
-      </c>
-      <c r="F25">
+      <c r="D25" s="10">
+        <v>296.44</v>
+      </c>
+      <c r="E25" s="10">
+        <v>289</v>
+      </c>
+      <c r="F25" s="10">
         <v>96.3</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="10">
         <v>96.03</v>
       </c>
       <c r="H25">
@@ -1195,22 +1203,22 @@
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="10">
         <v>6</v>
       </c>
-      <c r="D26">
-        <v>259.79000000000002</v>
-      </c>
-      <c r="E26">
-        <v>261.97000000000003</v>
-      </c>
-      <c r="F26">
+      <c r="D26" s="10">
+        <v>244.33</v>
+      </c>
+      <c r="E26" s="10">
+        <v>244.85</v>
+      </c>
+      <c r="F26" s="10">
         <v>112.58</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="10">
         <v>115.12</v>
       </c>
       <c r="H26">
@@ -1221,23 +1229,23 @@
       <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27">
+      <c r="C27" s="10">
+        <v>7</v>
+      </c>
+      <c r="D27" s="10">
         <v>290.12</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="10">
         <v>289.36</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="10">
         <v>80.77</v>
       </c>
-      <c r="G27">
-        <v>69.48</v>
+      <c r="G27" s="10">
+        <v>65.53</v>
       </c>
       <c r="H27">
         <v>45.08</v>

</xml_diff>